<commit_message>
done functions var 5 task 1
</commit_message>
<xml_diff>
--- a/Задания по Экселю/Диаграммы/Задание_1.xlsx
+++ b/Задания по Экселю/Диаграммы/Задание_1.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="17670" windowHeight="11070" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="17670" windowHeight="11070"/>
   </bookViews>
   <sheets>
-    <sheet name="Функция y" sheetId="1" r:id="rId1"/>
-    <sheet name="Функция g" sheetId="2" r:id="rId2"/>
-    <sheet name="Функция z" sheetId="3" r:id="rId3"/>
+    <sheet name="Вар. 5" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
@@ -25,6 +23,15 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>Функция y</t>
+  </si>
+  <si>
+    <t>Функция z</t>
+  </si>
+  <si>
+    <t>Функция g</t>
   </si>
 </sst>
 </file>
@@ -83,10 +90,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -388,191 +398,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>-3</v>
       </c>
-      <c r="B2" s="1">
-        <f>SQRT(1 + EXP(3 * A2))</f>
-        <v>1.0000617029984133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="B4" s="1">
+        <f>(1 + EXP(3 * A4))^(1/4)</f>
+        <v>1.0000308510233138</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(D4&lt;=0, (3+SIN(D4))/(1+(D4^2)), 2*(D4^2)*COS(D4)^2)</f>
+        <v>0.28588799919401325</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="H4" s="1">
+        <f>IF(  G4&lt;0,    (ABS(G4))^1/3,    IF(G4&gt;=1,   (ABS(3-G4))/(1+G4),    -2*G4+(G4)/(1+G4))     )</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>-2</v>
       </c>
-      <c r="B3" s="1">
-        <f>SQRT(1 + EXP(3 * A3))</f>
-        <v>1.0012386090121905</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="B5" s="1">
+        <f>(1 + EXP(3 * A5))^(1/4)</f>
+        <v>1.0006191128557311</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E10" si="0">IF(D5&lt;=0, (3+SIN(D5))/(1+(D5^2)), 2*(D5^2)*COS(D5)^2)</f>
+        <v>0.41814051463486362</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H10" si="1">IF(  G5&lt;0,    (ABS(G5))^1/3,    IF(G5&gt;=1,   (ABS(3-G5))/(1+G5),    -2*G5+(G5)/(1+G5))     )</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>-1</v>
       </c>
-      <c r="B4" s="1">
-        <f>SQRT(1 + EXP(3 * A4))</f>
-        <v>1.0245911713302354</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <f>SQRT(1 + EXP(3 * A5))</f>
-        <v>1.4142135623730951</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="B6" s="1">
+        <f>(1 + EXP(3 * A6))^(1/4)</f>
+        <v>1.0122209103403443</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0792645075960516</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <f>(1 + EXP(3 * A7))^(1/4)</f>
+        <v>1.189207115002721</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1">
-        <f>SQRT(1 + EXP(3 * A6))</f>
-        <v>4.5918990541155917</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="B8" s="1">
+        <f>(1 + EXP(3 * A8))^(1/4)</f>
+        <v>2.1428716840062059</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.58385316345285776</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <f>SQRT(1 + EXP(3 * A7))</f>
-        <v>20.110415050235414</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="B9" s="1">
+        <f>(1 + EXP(3 * A9))^(1/4)</f>
+        <v>4.4844637416569011</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3854255165455525</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="B8" s="1">
-        <f>SQRT(1 + EXP(3 * A8))</f>
-        <v>90.022685627431628</v>
+      <c r="B10" s="1">
+        <f>(1 + EXP(3 * A10))^(1/4)</f>
+        <v>9.4880285427180091</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>17.641532579853294</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>-3</v>
-      </c>
-      <c r="B2" s="1">
-        <f>IF(A2&lt;=0, (3+SIN(A2))/(1+A2^2), 2*A2^2*COS(A2)^2)</f>
-        <v>0.28588799919401325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>-2</v>
-      </c>
-      <c r="B3" s="1">
-        <f>IF(A3&lt;=0, (3+SIN(A3))/(1+A3^2), 2*A3^2*COS(A3)^2)</f>
-        <v>0.41814051463486362</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="B4" s="1">
-        <f>IF(A4&lt;=0, (3+SIN(A4))/(1+A4^2), 2*A4^2*COS(A4)^2)</f>
-        <v>1.0792645075960516</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <f>IF(A5&lt;=0, (3+SIN(A5))/(1+A5^2), 2*A5^2*COS(A5)^2)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <f>IF(A6&lt;=0, (3+SIN(A6))/(1+A6^2), 2*A6^2*COS(A6)^2)</f>
-        <v>0.58385316345285776</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <f>IF(A7&lt;=0, (3+SIN(A7))/(1+A7^2), 2*A7^2*COS(A7)^2)</f>
-        <v>1.3854255165455525</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <f>IF(A8&lt;=0, (3+SIN(A8))/(1+A8^2), 2*A8^2*COS(A8)^2)</f>
-        <v>17.641532579853294</v>
-      </c>
-    </row>
-  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="20000" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
diagrams var 6 task 1 done
</commit_message>
<xml_diff>
--- a/Задания по Экселю/Диаграммы/Задание_1.xlsx
+++ b/Задания по Экселю/Диаграммы/Задание_1.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="17670" windowHeight="11070"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="17670" windowHeight="11070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Вар. 5" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
@@ -400,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -451,7 +452,7 @@
         <v>-3</v>
       </c>
       <c r="B4" s="1">
-        <f>(1 + EXP(3 * A4))^(1/4)</f>
+        <f t="shared" ref="B4:B10" si="0">(1 + EXP(3 * A4))^(1/4)</f>
         <v>1.0000308510233138</v>
       </c>
       <c r="D4" s="1">
@@ -474,21 +475,21 @@
         <v>-2</v>
       </c>
       <c r="B5" s="1">
-        <f>(1 + EXP(3 * A5))^(1/4)</f>
+        <f t="shared" si="0"/>
         <v>1.0006191128557311</v>
       </c>
       <c r="D5" s="1">
         <v>-2</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E10" si="0">IF(D5&lt;=0, (3+SIN(D5))/(1+(D5^2)), 2*(D5^2)*COS(D5)^2)</f>
+        <f t="shared" ref="E5:E10" si="1">IF(D5&lt;=0, (3+SIN(D5))/(1+(D5^2)), 2*(D5^2)*COS(D5)^2)</f>
         <v>0.41814051463486362</v>
       </c>
       <c r="G5" s="1">
         <v>-2</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:H10" si="1">IF(  G5&lt;0,    (ABS(G5))^1/3,    IF(G5&gt;=1,   (ABS(3-G5))/(1+G5),    -2*G5+(G5)/(1+G5))     )</f>
+        <f t="shared" ref="H5:H10" si="2">IF(  G5&lt;0,    (ABS(G5))^1/3,    IF(G5&gt;=1,   (ABS(3-G5))/(1+G5),    -2*G5+(G5)/(1+G5))     )</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -497,21 +498,21 @@
         <v>-1</v>
       </c>
       <c r="B6" s="1">
-        <f>(1 + EXP(3 * A6))^(1/4)</f>
+        <f t="shared" si="0"/>
         <v>1.0122209103403443</v>
       </c>
       <c r="D6" s="1">
         <v>-1</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0792645075960516</v>
       </c>
       <c r="G6" s="1">
         <v>-1</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -520,21 +521,21 @@
         <v>0</v>
       </c>
       <c r="B7" s="1">
-        <f>(1 + EXP(3 * A7))^(1/4)</f>
+        <f t="shared" si="0"/>
         <v>1.189207115002721</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -543,21 +544,21 @@
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <f>(1 + EXP(3 * A8))^(1/4)</f>
+        <f t="shared" si="0"/>
         <v>2.1428716840062059</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.58385316345285776</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -566,21 +567,21 @@
         <v>2</v>
       </c>
       <c r="B9" s="1">
-        <f>(1 + EXP(3 * A9))^(1/4)</f>
+        <f t="shared" si="0"/>
         <v>4.4844637416569011</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3854255165455525</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -589,21 +590,21 @@
         <v>3</v>
       </c>
       <c r="B10" s="1">
-        <f>(1 + EXP(3 * A10))^(1/4)</f>
+        <f t="shared" si="0"/>
         <v>9.4880285427180091</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.641532579853294</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -616,4 +617,222 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="20000" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="B4" s="1">
+        <f>((1 + A4 * EXP(- A4)))/2+ SQRT((A4^2)+SIN(A4)^2)</f>
+        <v>-26.624988076091856</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(D4&lt;=0,  SQRT(1+ABS(D4)),  (1+3*D4)/2+(1+D4)^1/3  )</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="H4" s="1">
+        <f>IF(  G4&lt;0,    (ABS(G4))^1/3,    IF(G4&gt;=1,   (ABS(3-G4))/(1+G4),    -2*G4+(G4)/(1+G4))     )</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:B10" si="0">((1 + A5 * EXP(- A5)))/2+ SQRT((A5^2)+SIN(A5)^2)</f>
+        <v>-4.6920531834952142</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E10" si="1">IF(D5&lt;=0,  SQRT(1+ABS(D5)),  (1+3*D5)/2+(1+D5)^1/3  )</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H10" si="2">IF(  G5&lt;0,    (ABS(G5))^1/3,    IF(G5&gt;=1,   (ABS(3-G5))/(1+G5),    -2*G5+(G5)/(1+G5))     )</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.44779191429441156</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9908725491096553</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8323381986720491</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5779979112414417</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>